<commit_message>
Free function interface make_index modified
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -19,7 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3" count="3">
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
   <si>
     <t>mm</t>
   </si>
@@ -82,10 +88,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -104,19 +110,15 @@
           <t>b</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
+      <c r="C1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
+      <c r="A2">
+        <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
@@ -124,14 +126,25 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75">
-      <c r="A3" t="s">
-        <v>0</v>
+      <c r="A3">
+        <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
         <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3.2999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>